<commit_message>
调整配置表Card Dialog Friend FriendFavor 新增CardAptitudeUp卡牌资质升级配置
</commit_message>
<xml_diff>
--- a/common/Card.xlsx
+++ b/common/Card.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
   <si>
     <t>序号</t>
   </si>
@@ -29,6 +29,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">品质
 </t>
     </r>
@@ -93,6 +100,9 @@
     <t>技能id_2</t>
   </si>
   <si>
+    <t>兑换所需碎片</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -403,6 +413,31 @@
       </rPr>
       <t xml:space="preserve">skill_id_2
 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>int</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>piece_num</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -432,9 +467,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -458,6 +493,75 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -466,7 +570,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -480,125 +607,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -637,181 +672,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,8 +891,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -877,6 +942,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -887,21 +961,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -918,30 +977,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -958,10 +993,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -970,137 +1005,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1114,6 +1149,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1443,10 +1484,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelRow="2"/>
@@ -1459,10 +1500,12 @@
     <col min="7" max="10" width="10.875" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.625" style="1" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="13" max="14" width="9" style="1"/>
+    <col min="15" max="15" width="11.125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="98.25" spans="1:14">
+    <row r="1" ht="98.25" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1505,63 +1548,69 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" ht="32.25" spans="1:14">
+    <row r="2" ht="33.75" spans="1:15">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="K2" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="L2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="N2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>301001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -1591,6 +1640,9 @@
         <v>0</v>
       </c>
       <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>